<commit_message>
wait and new page
</commit_message>
<xml_diff>
--- a/Excel_File/TestData.xlsx
+++ b/Excel_File/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFBF89D-F1EF-4DDE-B4D1-C39346FCA4A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A061A963-566E-415C-B58E-3F722A2BE511}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="3405" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>admin123</t>
   </si>
@@ -28,10 +28,16 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>prasad</t>
-  </si>
-  <si>
-    <t>Fail</t>
+    <t>VLSI</t>
+  </si>
+  <si>
+    <t>Chip Designer</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>DEO</t>
   </si>
 </sst>
 </file>
@@ -434,26 +440,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1">
-        <v>123456</v>
-      </c>
-      <c r="D1">
-        <v>123456</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comments and log updated
</commit_message>
<xml_diff>
--- a/Excel_File/TestData.xlsx
+++ b/Excel_File/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{568D6B07-6922-439F-8653-7E4E9104C50B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8B1BE3-BAE9-41C5-AA35-30918321B8B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13665" windowHeight="3645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13665" windowHeight="3645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,11 @@
     <sheet name="Sal" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>admin123</t>
   </si>
@@ -26,22 +25,16 @@
     <t>admin</t>
   </si>
   <si>
-    <t>Chip Designer</t>
-  </si>
-  <si>
-    <t>DEO</t>
-  </si>
-  <si>
     <t>Spe Incr</t>
   </si>
   <si>
-    <t>JobCD6</t>
-  </si>
-  <si>
-    <t>JobDE6</t>
-  </si>
-  <si>
-    <t>Pass</t>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>QA12</t>
+  </si>
+  <si>
+    <t>QA12D</t>
   </si>
 </sst>
 </file>
@@ -434,7 +427,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -444,31 +437,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -480,7 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -488,7 +475,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comments, spaces removed and apply file created
</commit_message>
<xml_diff>
--- a/Excel_File/TestData.xlsx
+++ b/Excel_File/TestData.xlsx
@@ -1,46 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D834ACA1-4107-4F10-9A2D-71E277074678}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031D49E8-55CD-465F-A9A8-ACC77F02239B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13665" windowHeight="3645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="AddVacy" sheetId="2" r:id="rId2"/>
-    <sheet name="Sal" sheetId="3" r:id="rId3"/>
+    <sheet name="Job" sheetId="2" r:id="rId2"/>
+    <sheet name="Leave" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+  <si>
+    <t>admin</t>
+  </si>
   <si>
     <t>admin123</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Spe Incr</t>
+    <t>cyber1</t>
+  </si>
+  <si>
+    <t>cyber</t>
   </si>
   <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>QA2</t>
-  </si>
-  <si>
-    <t>QA2D</t>
-  </si>
-  <si>
-    <t>Success</t>
-  </si>
-  <si>
-    <t>Fail</t>
+    <t>Job Title Already exit</t>
   </si>
 </sst>
 </file>
@@ -425,15 +419,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -446,7 +440,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,24 +452,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -488,17 +482,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Salary Comp file added
</commit_message>
<xml_diff>
--- a/Excel_File/TestData.xlsx
+++ b/Excel_File/TestData.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031D49E8-55CD-465F-A9A8-ACC77F02239B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712529B2-D3A8-4F16-9EC8-7C863C6EAE1F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Job" sheetId="2" r:id="rId2"/>
-    <sheet name="Leave" sheetId="3" r:id="rId3"/>
+    <sheet name="SalComp" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>admin</t>
   </si>
@@ -25,16 +25,19 @@
     <t>admin123</t>
   </si>
   <si>
-    <t>cyber1</t>
-  </si>
-  <si>
-    <t>cyber</t>
+    <t>Cyber 15</t>
+  </si>
+  <si>
+    <t>Cyber 46</t>
+  </si>
+  <si>
+    <t>cyber 46</t>
   </si>
   <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>Job Title Already exit</t>
+    <t>Food All2</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +430,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -437,10 +440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,21 +458,15 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -481,12 +478,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Log and Excel Updated
</commit_message>
<xml_diff>
--- a/Excel_File/TestData.xlsx
+++ b/Excel_File/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712529B2-D3A8-4F16-9EC8-7C863C6EAE1F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15D2883-9FFB-4327-ABC6-41D6C705FE65}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>admin</t>
   </si>
@@ -34,10 +34,19 @@
     <t>cyber 46</t>
   </si>
   <si>
+    <t>Food All3</t>
+  </si>
+  <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>Food All2</t>
+    <t>Job Title Already exit</t>
+  </si>
+  <si>
+    <t>Job Submitted</t>
+  </si>
+  <si>
+    <t>Already exit</t>
   </si>
 </sst>
 </file>
@@ -416,13 +425,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +439,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -440,10 +449,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,6 +469,9 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -467,6 +479,9 @@
       </c>
       <c r="B2" t="s">
         <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -476,15 +491,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dynamic reports and screenshots
</commit_message>
<xml_diff>
--- a/Excel_File/TestData.xlsx
+++ b/Excel_File/TestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="10">
   <si>
     <t>admin</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Job Submitted</t>
+  </si>
+  <si>
+    <t>Job Title Already exit</t>
   </si>
 </sst>
 </file>
@@ -443,7 +449,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
@@ -463,6 +469,9 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -470,6 +479,9 @@
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>